<commit_message>
tests on WPS and static configuration done by Chiebao
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan_20200826_cellini.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan_20200826_cellini.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_His." sheetId="3" r:id="rId1"/>
@@ -805,7 +805,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="286">
   <si>
     <t>Test ID</t>
   </si>
@@ -2156,7 +2156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2258,6 +2258,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -4360,7 +4365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -7404,8 +7409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7417,7 +7422,7 @@
     <col min="5" max="5" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -7676,11 +7681,18 @@
       <c r="D11" s="16" t="s">
         <v>144</v>
       </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="49">
+        <v>44075</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
@@ -7696,11 +7708,18 @@
       <c r="D12" s="16" t="s">
         <v>202</v>
       </c>
+      <c r="E12" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="51">
+        <v>44075</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
@@ -7716,8 +7735,15 @@
       <c r="D13" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="49">
+        <v>44076</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
@@ -9626,7 +9652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>